<commit_message>
Update to run specific tests with runable
</commit_message>
<xml_diff>
--- a/MavenTestProject3/src/main/java/dataEngine/DataEngine1.xlsx
+++ b/MavenTestProject3/src/main/java/dataEngine/DataEngine1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="46">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -517,8 +517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -549,7 +549,7 @@
         <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>45</v>
@@ -563,7 +563,7 @@
         <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
         <v>45</v>
@@ -605,7 +605,7 @@
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
@@ -633,7 +633,7 @@
         <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
@@ -646,10 +646,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -956,6 +956,147 @@
         <v>34</v>
       </c>
       <c r="E19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B24" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" t="s">
+        <v>31</v>
+      </c>
+      <c r="D27" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="E28" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Making grid compatible with Edge
</commit_message>
<xml_diff>
--- a/MavenTestProject3/src/main/java/dataEngine/DataEngine1.xlsx
+++ b/MavenTestProject3/src/main/java/dataEngine/DataEngine1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium Files\Git Project\MavenTestProject3\src\main\java\dataEngine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\winms\IdeaProjects\selenium-poc\MavenTestProject3\src\main\java\dataEngine\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
   <si>
     <t>TestCaseID</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>FireFox</t>
+  </si>
+  <si>
+    <t>Edge</t>
   </si>
 </sst>
 </file>
@@ -508,8 +511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,10 +543,10 @@
         <v>36</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -568,7 +571,7 @@
         <v>36</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
         <v>42</v>
@@ -639,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>

</xml_diff>